<commit_message>
Parse simple colours out of the xlsx if the cell is blank in a data row
</commit_message>
<xml_diff>
--- a/test/sample-inputs/Brews.xlsx
+++ b/test/sample-inputs/Brews.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>name</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t>american amber</t>
+  </si>
+  <si>
+    <t>colour</t>
   </si>
 </sst>
 </file>
@@ -63,12 +66,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC600AE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -83,14 +98,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFC600AE"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -362,13 +384,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -378,8 +402,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -389,8 +416,9 @@
       <c r="C2">
         <v>8</v>
       </c>
+      <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -400,6 +428,7 @@
       <c r="C3">
         <v>9</v>
       </c>
+      <c r="D3" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>